<commit_message>
Change on GamePanel ANd EventSystem
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/__enums__.xlsx
+++ b/Luban/Config/Datas/__enums__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07937091-32E3-4100-A751-84944C5E2F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7018DD-670D-433D-83B9-CEB75E0626FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="3090" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3930" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DIESON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>属性成长</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -159,6 +155,10 @@
   </si>
   <si>
     <t>下一代获得新的事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIE_SON</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -500,7 +500,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -609,7 +609,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -617,7 +617,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -625,47 +625,47 @@
         <v>26</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>